<commit_message>
primer forms de pedidos
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/inventarios.xlsx
+++ b/ProyectoPooDist/excels/inventarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Nombre</t>
   </si>
@@ -56,10 +56,13 @@
     <t>Ponedora Fase 1</t>
   </si>
   <si>
-    <t>Miamix</t>
-  </si>
-  <si>
-    <t>Manuel</t>
+    <t>Gatimar</t>
+  </si>
+  <si>
+    <t>Hill</t>
+  </si>
+  <si>
+    <t>Ponedora Fase 2</t>
   </si>
 </sst>
 </file>
@@ -104,7 +107,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -237,13 +240,30 @@
         <v>15</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>500.0</v>
+        <v>10.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>123.0</v>
+        <v>3.0</v>
       </c>
       <c r="E8" t="n" s="0">
         <v>14.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C9" t="n" s="0">
+        <v>256.0</v>
+      </c>
+      <c r="D9" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E9" t="n" s="0">
+        <v>30.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
control viajes modificacion completa
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/inventarios.xlsx
+++ b/ProyectoPooDist/excels/inventarios.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Nombre</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>Ponedora Fase 2</t>
+  </si>
+  <si>
+    <t>Super Vaca Lechera</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -144,7 +147,7 @@
         <v>3.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>212.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="3">
@@ -161,7 +164,7 @@
         <v>3.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>300.0</v>
+        <v>1150.0</v>
       </c>
     </row>
     <row r="4">
@@ -178,7 +181,7 @@
         <v>3.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>1050.0</v>
+        <v>1515.0</v>
       </c>
     </row>
     <row r="5">
@@ -195,7 +198,7 @@
         <v>3.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>300.0</v>
+        <v>10150.0</v>
       </c>
     </row>
     <row r="6">
@@ -212,7 +215,7 @@
         <v>3.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>450.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="7">
@@ -229,7 +232,7 @@
         <v>3.0</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>310.0</v>
+        <v>1150.0</v>
       </c>
     </row>
     <row r="8">
@@ -246,7 +249,7 @@
         <v>3.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>164.0</v>
+        <v>150.0</v>
       </c>
     </row>
     <row r="9">
@@ -263,7 +266,24 @@
         <v>3.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>180.0</v>
+        <v>115.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="C10" t="n" s="0">
+        <v>160.0</v>
+      </c>
+      <c r="D10" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="E10" t="n" s="0">
+        <v>150.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
funciones de clientes y de ventas conclusidas casi en su totalidad
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/inventarios.xlsx
+++ b/ProyectoPooDist/excels/inventarios.xlsx
@@ -141,7 +141,7 @@
         <v>3.0</v>
       </c>
       <c r="E2" t="n" s="0">
-        <v>0.0</v>
+        <v>962.0</v>
       </c>
     </row>
     <row r="3">
@@ -158,7 +158,7 @@
         <v>3.0</v>
       </c>
       <c r="E3" t="n" s="0">
-        <v>150.0</v>
+        <v>607.0</v>
       </c>
     </row>
     <row r="4">
@@ -175,7 +175,7 @@
         <v>3.0</v>
       </c>
       <c r="E4" t="n" s="0">
-        <v>900.0</v>
+        <v>803.0</v>
       </c>
     </row>
     <row r="5">
@@ -192,7 +192,7 @@
         <v>3.0</v>
       </c>
       <c r="E5" t="n" s="0">
-        <v>150.0</v>
+        <v>963.0</v>
       </c>
     </row>
     <row r="6">
@@ -209,7 +209,7 @@
         <v>3.0</v>
       </c>
       <c r="E6" t="n" s="0">
-        <v>300.0</v>
+        <v>925.0</v>
       </c>
     </row>
     <row r="7">
@@ -226,7 +226,7 @@
         <v>3.0</v>
       </c>
       <c r="E7" t="n" s="0">
-        <v>160.0</v>
+        <v>935.0</v>
       </c>
     </row>
     <row r="8">
@@ -243,7 +243,7 @@
         <v>123.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>314.0</v>
+        <v>999.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>